<commit_message>
Checking numbers for the bifurcation results section
</commit_message>
<xml_diff>
--- a/data/Other/excelSheet/Fig1/Fig1DE.xlsx
+++ b/data/Other/excelSheet/Fig1/Fig1DE.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="25">
   <si>
     <t>treeIndex</t>
   </si>
@@ -120,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="81">
+  <borders count="101">
     <border>
       <left/>
       <right/>
@@ -208,11 +208,31 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -294,6 +314,26 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="99" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="100" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,18 +360,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="93" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="93" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -342,7 +382,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="93" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -353,7 +393,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="93" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -364,7 +404,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="93" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -375,7 +415,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="93" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -386,7 +426,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="93" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -397,7 +437,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="93" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -408,7 +448,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="93" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -419,7 +459,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="93" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -430,7 +470,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="93" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -441,7 +481,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="93" t="s">
         <v>23</v>
       </c>
       <c r="B12">
@@ -466,18 +506,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="95" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="95" t="s">
         <v>13</v>
       </c>
       <c r="B2">
@@ -488,7 +528,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="95" t="s">
         <v>14</v>
       </c>
       <c r="B3">
@@ -499,7 +539,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="95" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -510,7 +550,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="95" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -521,7 +561,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="95" t="s">
         <v>17</v>
       </c>
       <c r="B6">
@@ -532,7 +572,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="95" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -543,7 +583,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="95" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -554,7 +594,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="95" t="s">
         <v>20</v>
       </c>
       <c r="B9">
@@ -565,7 +605,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="95" t="s">
         <v>21</v>
       </c>
       <c r="B10">
@@ -576,7 +616,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="95" t="s">
         <v>22</v>
       </c>
       <c r="B11">
@@ -587,7 +627,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="95" t="s">
         <v>24</v>
       </c>
       <c r="B12">
@@ -612,18 +652,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="97" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="97" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -634,7 +674,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -645,7 +685,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="97" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -656,7 +696,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="97" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -667,7 +707,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="97" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -678,7 +718,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="97" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -689,7 +729,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="97" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -700,7 +740,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -711,7 +751,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="97" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -722,7 +762,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="97" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -733,7 +773,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="97" t="s">
         <v>1</v>
       </c>
       <c r="B12">
@@ -744,7 +784,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B13">
@@ -755,7 +795,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="97" t="s">
         <v>3</v>
       </c>
       <c r="B14">
@@ -766,7 +806,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="97" t="s">
         <v>4</v>
       </c>
       <c r="B15">
@@ -777,7 +817,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="97" t="s">
         <v>5</v>
       </c>
       <c r="B16">
@@ -788,7 +828,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="97" t="s">
         <v>6</v>
       </c>
       <c r="B17">
@@ -799,7 +839,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="97" t="s">
         <v>7</v>
       </c>
       <c r="B18">
@@ -810,7 +850,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B19">
@@ -821,7 +861,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="97" t="s">
         <v>9</v>
       </c>
       <c r="B20">
@@ -832,7 +872,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="97" t="s">
         <v>10</v>
       </c>
       <c r="B21">
@@ -843,7 +883,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="97" t="s">
         <v>1</v>
       </c>
       <c r="B22">
@@ -854,7 +894,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B23">
@@ -865,7 +905,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="97" t="s">
         <v>3</v>
       </c>
       <c r="B24">
@@ -876,7 +916,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="97" t="s">
         <v>4</v>
       </c>
       <c r="B25">
@@ -887,7 +927,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="97" t="s">
         <v>5</v>
       </c>
       <c r="B26">
@@ -898,7 +938,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="97" t="s">
         <v>6</v>
       </c>
       <c r="B27">
@@ -909,7 +949,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="97" t="s">
         <v>7</v>
       </c>
       <c r="B28">
@@ -920,7 +960,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B29">
@@ -931,7 +971,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="97" t="s">
         <v>9</v>
       </c>
       <c r="B30">
@@ -942,7 +982,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="97" t="s">
         <v>10</v>
       </c>
       <c r="B31">
@@ -953,7 +993,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="97" t="s">
         <v>1</v>
       </c>
       <c r="B32">
@@ -964,7 +1004,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="97" t="s">
         <v>2</v>
       </c>
       <c r="B33">
@@ -975,7 +1015,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="97" t="s">
         <v>3</v>
       </c>
       <c r="B34">
@@ -986,7 +1026,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="97" t="s">
         <v>4</v>
       </c>
       <c r="B35">
@@ -997,7 +1037,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="77" t="s">
+      <c r="A36" s="97" t="s">
         <v>5</v>
       </c>
       <c r="B36">
@@ -1008,7 +1048,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="77" t="s">
+      <c r="A37" s="97" t="s">
         <v>6</v>
       </c>
       <c r="B37">
@@ -1019,7 +1059,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="97" t="s">
         <v>7</v>
       </c>
       <c r="B38">
@@ -1030,7 +1070,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="77" t="s">
+      <c r="A39" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B39">
@@ -1041,7 +1081,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="97" t="s">
         <v>9</v>
       </c>
       <c r="B40">
@@ -1052,7 +1092,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="77" t="s">
+      <c r="A41" s="97" t="s">
         <v>10</v>
       </c>
       <c r="B41">
@@ -1063,7 +1103,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="77" t="s">
+      <c r="A42" s="97" t="s">
         <v>23</v>
       </c>
       <c r="B42">
@@ -1088,18 +1128,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="99" t="s">
         <v>13</v>
       </c>
       <c r="B2">
@@ -1110,7 +1150,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="99" t="s">
         <v>14</v>
       </c>
       <c r="B3">
@@ -1121,7 +1161,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="99" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -1132,7 +1172,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="99" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -1143,7 +1183,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="99" t="s">
         <v>17</v>
       </c>
       <c r="B6">
@@ -1154,7 +1194,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="99" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -1165,7 +1205,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="99" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -1176,7 +1216,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="99" t="s">
         <v>20</v>
       </c>
       <c r="B9">
@@ -1187,7 +1227,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B10">
@@ -1198,7 +1238,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="99" t="s">
         <v>22</v>
       </c>
       <c r="B11">
@@ -1209,7 +1249,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="99" t="s">
         <v>13</v>
       </c>
       <c r="B12">
@@ -1220,7 +1260,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="99" t="s">
         <v>14</v>
       </c>
       <c r="B13">
@@ -1231,7 +1271,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="99" t="s">
         <v>15</v>
       </c>
       <c r="B14">
@@ -1242,7 +1282,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="99" t="s">
         <v>16</v>
       </c>
       <c r="B15">
@@ -1253,7 +1293,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="79" t="s">
+      <c r="A16" s="99" t="s">
         <v>17</v>
       </c>
       <c r="B16">
@@ -1264,7 +1304,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="99" t="s">
         <v>18</v>
       </c>
       <c r="B17">
@@ -1275,7 +1315,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="99" t="s">
         <v>19</v>
       </c>
       <c r="B18">
@@ -1286,7 +1326,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="99" t="s">
         <v>20</v>
       </c>
       <c r="B19">
@@ -1297,7 +1337,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="79" t="s">
+      <c r="A20" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B20">
@@ -1308,7 +1348,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="99" t="s">
         <v>22</v>
       </c>
       <c r="B21">
@@ -1319,7 +1359,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="99" t="s">
         <v>13</v>
       </c>
       <c r="B22">
@@ -1330,7 +1370,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="99" t="s">
         <v>14</v>
       </c>
       <c r="B23">
@@ -1341,7 +1381,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="99" t="s">
         <v>15</v>
       </c>
       <c r="B24">
@@ -1352,7 +1392,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="99" t="s">
         <v>16</v>
       </c>
       <c r="B25">
@@ -1363,7 +1403,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="99" t="s">
         <v>17</v>
       </c>
       <c r="B26">
@@ -1374,7 +1414,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="99" t="s">
         <v>18</v>
       </c>
       <c r="B27">
@@ -1385,7 +1425,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="99" t="s">
         <v>19</v>
       </c>
       <c r="B28">
@@ -1396,7 +1436,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="99" t="s">
         <v>20</v>
       </c>
       <c r="B29">
@@ -1407,7 +1447,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="79" t="s">
+      <c r="A30" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B30">
@@ -1418,7 +1458,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="79" t="s">
+      <c r="A31" s="99" t="s">
         <v>22</v>
       </c>
       <c r="B31">
@@ -1429,7 +1469,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="99" t="s">
         <v>13</v>
       </c>
       <c r="B32">
@@ -1440,7 +1480,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="99" t="s">
         <v>14</v>
       </c>
       <c r="B33">
@@ -1451,7 +1491,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="99" t="s">
         <v>15</v>
       </c>
       <c r="B34">
@@ -1462,7 +1502,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="99" t="s">
         <v>16</v>
       </c>
       <c r="B35">
@@ -1473,7 +1513,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="79" t="s">
+      <c r="A36" s="99" t="s">
         <v>17</v>
       </c>
       <c r="B36">
@@ -1484,7 +1524,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="79" t="s">
+      <c r="A37" s="99" t="s">
         <v>18</v>
       </c>
       <c r="B37">
@@ -1495,7 +1535,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="79" t="s">
+      <c r="A38" s="99" t="s">
         <v>19</v>
       </c>
       <c r="B38">
@@ -1506,7 +1546,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="79" t="s">
+      <c r="A39" s="99" t="s">
         <v>20</v>
       </c>
       <c r="B39">
@@ -1517,7 +1557,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="79" t="s">
+      <c r="A40" s="99" t="s">
         <v>21</v>
       </c>
       <c r="B40">
@@ -1528,7 +1568,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="99" t="s">
         <v>22</v>
       </c>
       <c r="B41">
@@ -1539,7 +1579,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="79" t="s">
+      <c r="A42" s="99" t="s">
         <v>24</v>
       </c>
       <c r="B42">
@@ -1580,18 +1620,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="81" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="81" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1602,7 +1642,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="81" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1613,7 +1653,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="81" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1624,7 +1664,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="81" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1635,7 +1675,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="81" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1646,7 +1686,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="81" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1657,7 +1697,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="81" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1668,7 +1708,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="81" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1679,7 +1719,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="81" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1690,7 +1730,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="81" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1715,18 +1755,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="83" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="83" t="s">
         <v>13</v>
       </c>
       <c r="B2">
@@ -1737,7 +1777,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="83" t="s">
         <v>14</v>
       </c>
       <c r="B3">
@@ -1748,7 +1788,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="83" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -1759,7 +1799,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="83" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -1770,7 +1810,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="83" t="s">
         <v>17</v>
       </c>
       <c r="B6">
@@ -1781,7 +1821,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="83" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -1792,7 +1832,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="83" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -1803,7 +1843,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="83" t="s">
         <v>20</v>
       </c>
       <c r="B9">
@@ -1814,7 +1854,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="83" t="s">
         <v>21</v>
       </c>
       <c r="B10">
@@ -1825,7 +1865,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="83" t="s">
         <v>22</v>
       </c>
       <c r="B11">
@@ -1850,18 +1890,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="85" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1872,7 +1912,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="85" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -1883,7 +1923,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="85" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -1894,7 +1934,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="85" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -1905,7 +1945,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="85" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -1916,7 +1956,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="85" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -1927,7 +1967,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="85" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -1938,7 +1978,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="85" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -1949,7 +1989,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="85" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -1960,7 +2000,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="85" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -1985,18 +2025,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="87" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="87" t="s">
         <v>13</v>
       </c>
       <c r="B2">
@@ -2007,7 +2047,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="87" t="s">
         <v>14</v>
       </c>
       <c r="B3">
@@ -2018,7 +2058,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="87" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -2029,7 +2069,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="87" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -2040,7 +2080,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="87" t="s">
         <v>17</v>
       </c>
       <c r="B6">
@@ -2051,7 +2091,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="87" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -2062,7 +2102,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="87" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -2073,7 +2113,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="87" t="s">
         <v>20</v>
       </c>
       <c r="B9">
@@ -2084,7 +2124,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="87" t="s">
         <v>21</v>
       </c>
       <c r="B10">
@@ -2095,7 +2135,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="87" t="s">
         <v>22</v>
       </c>
       <c r="B11">
@@ -2120,18 +2160,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="89" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="89" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -2142,7 +2182,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2153,7 +2193,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="89" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -2164,7 +2204,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="89" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -2175,7 +2215,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="89" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -2186,7 +2226,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="89" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -2197,7 +2237,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="89" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -2208,7 +2248,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="89" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -2219,7 +2259,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="89" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -2230,7 +2270,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="89" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -2255,18 +2295,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="91" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="91" t="s">
         <v>13</v>
       </c>
       <c r="B2">
@@ -2277,7 +2317,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="91" t="s">
         <v>14</v>
       </c>
       <c r="B3">
@@ -2288,7 +2328,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="91" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -2299,7 +2339,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="91" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -2310,7 +2350,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="91" t="s">
         <v>17</v>
       </c>
       <c r="B6">
@@ -2321,7 +2361,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="91" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -2332,7 +2372,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="91" t="s">
         <v>19</v>
       </c>
       <c r="B8">
@@ -2343,7 +2383,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="91" t="s">
         <v>20</v>
       </c>
       <c r="B9">
@@ -2354,7 +2394,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="91" t="s">
         <v>21</v>
       </c>
       <c r="B10">
@@ -2365,7 +2405,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="91" t="s">
         <v>22</v>
       </c>
       <c r="B11">

</xml_diff>